<commit_message>
Diccionario de Datos db
Documentacion del Proyecto
</commit_message>
<xml_diff>
--- a/Documentacion del Proyecto/Diccionario de Datos Db/Diccionario de Datos.xlsx
+++ b/Documentacion del Proyecto/Diccionario de Datos Db/Diccionario de Datos.xlsx
@@ -388,12 +388,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -421,30 +415,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,436 +746,436 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>15</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>45</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>45</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>45</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>45</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>10</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="12">
         <v>10</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="12">
         <v>10</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="12">
         <v>10</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="11">
         <v>10</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="12">
         <v>10</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="12">
         <v>45</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="12">
         <v>10</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:C33"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:C20"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>